<commit_message>
Site updated: 2021-02-22 23:09:57
</commit_message>
<xml_diff>
--- a/appidlist.xlsx
+++ b/appidlist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB74338-682F-444D-8EDB-8641AEFF21DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81F279C-8748-1F42-A321-35C6812C3A73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="460" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -359,11 +359,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>密码在艾伲Lab</t>
+    <t>仅原始用户可获取密码</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>仅原始用户可获取密码</t>
+    <t>密码在艾伲Lab小程序</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -371,7 +371,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -383,6 +383,15 @@
       <sz val="9"/>
       <name val="等线"/>
       <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -407,8 +416,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -692,7 +702,7 @@
   <dimension ref="A1:B100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -703,18 +713,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B1" t="s">
-        <v>113</v>
-      </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>